<commit_message>
Added graph in xlsx file
</commit_message>
<xml_diff>
--- a/AODV_vs_DSR.xlsx
+++ b/AODV_vs_DSR.xlsx
@@ -336,7 +336,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1226,16 +1225,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1681162</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1563,7 +1562,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>